<commit_message>
Updating Core HForms and fixing db child table reference
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/extension-forms/xls/inmigration_ext.xlsx
+++ b/src/main/resources/samples/extension-forms/xls/inmigration_ext.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="26415" windowHeight="9870"/>
+    <workbookView windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="114">
   <si>
     <t>type</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Tipo de Imigração Externa</t>
+  </si>
+  <si>
+    <t>${migration_type}='XEN'</t>
   </si>
   <si>
     <t>custom_quest1</t>
@@ -365,10 +368,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -429,10 +432,24 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -452,9 +469,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -468,16 +492,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -491,42 +544,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -534,26 +552,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -596,7 +599,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,31 +737,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -644,61 +749,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,61 +767,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -775,24 +778,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -811,37 +796,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -875,150 +834,194 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1508,11 +1511,11 @@
   <dimension ref="A1:V55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5:B10"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
@@ -1528,7 +1531,8 @@
     <col min="9" max="9" width="24.5" style="17" customWidth="1"/>
     <col min="10" max="10" width="9" style="6"/>
     <col min="11" max="11" width="30.9083333333333" style="17" customWidth="1"/>
-    <col min="12" max="13" width="9" style="17"/>
+    <col min="12" max="12" width="9" style="17"/>
+    <col min="13" max="13" width="18.9083333333333" style="17" customWidth="1"/>
     <col min="14" max="14" width="9" style="6"/>
     <col min="15" max="15" width="9" style="17"/>
     <col min="16" max="16" width="10.75" style="17" customWidth="1"/>
@@ -1822,6 +1826,9 @@
       <c r="J10" s="39" t="s">
         <v>24</v>
       </c>
+      <c r="M10" s="27" t="s">
+        <v>48</v>
+      </c>
       <c r="N10" s="39" t="s">
         <v>24</v>
       </c>
@@ -1831,13 +1838,13 @@
         <v>27</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="J11" s="40"/>
       <c r="N11" s="40"/>
@@ -1847,13 +1854,13 @@
         <v>27</v>
       </c>
       <c r="B12" s="28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J12" s="40"/>
       <c r="N12" s="40"/>
@@ -2058,7 +2065,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6333333333333" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -2072,16 +2079,16 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1" spans="1:5">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>17</v>
@@ -2089,212 +2096,212 @@
     </row>
     <row r="2" ht="12.75" customHeight="1" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B2" s="8">
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="8">
         <v>0</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="11" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="13" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="11" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -3712,33 +3719,33 @@
   <sheetData>
     <row r="1" ht="15" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>

</xml_diff>